<commit_message>
Ajustes no Modelo e no versionamento
</commit_message>
<xml_diff>
--- a/AutoFillTS/Model/Modelo.xlsx
+++ b/AutoFillTS/Model/Modelo.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D453D428-29EC-4A7D-BC1C-41FDEF1ABCA2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo1" sheetId="1" r:id="rId1"/>
-    <sheet name="Modelo2" sheetId="3" r:id="rId2"/>
-    <sheet name="Parametros" sheetId="2" r:id="rId3"/>
+    <sheet name="Modelo2" sheetId="4" r:id="rId2"/>
+    <sheet name="Modelo3" sheetId="3" r:id="rId3"/>
+    <sheet name="Parametros" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Data</t>
   </si>
@@ -205,12 +207,15 @@
   </si>
   <si>
     <t>RTC</t>
+  </si>
+  <si>
+    <t>TFS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -324,7 +329,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -362,7 +367,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -397,6 +402,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -432,9 +454,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,10 +646,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
@@ -673,7 +712,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f ca="1">TODAY() - 3</f>
-        <v>42716</v>
+        <v>43298</v>
       </c>
       <c r="B2" s="2">
         <v>0.33333333333333331</v>
@@ -726,7 +765,7 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f ca="1">TODAY() - 2</f>
-        <v>42717</v>
+        <v>43299</v>
       </c>
       <c r="B3" s="2">
         <v>0.33333333333333331</v>
@@ -747,7 +786,7 @@
         <v>48</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H12" si="0" xml:space="preserve"> (C3 - B3) + (E3 - D3)</f>
+        <f t="shared" ref="H3" si="0" xml:space="preserve"> (C3 - B3) + (E3 - D3)</f>
         <v>0.33333333333333343</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -779,7 +818,7 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f ca="1">TODAY() - 1</f>
-        <v>42718</v>
+        <v>43300</v>
       </c>
       <c r="B4" s="2">
         <v>0.33333333333333331</v>
@@ -828,7 +867,7 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f ca="1">TODAY()</f>
-        <v>42719</v>
+        <v>43301</v>
       </c>
       <c r="B5" s="2">
         <v>0.33333333333333331</v>
@@ -1267,13 +1306,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Parametros!$F$2:$F$26</xm:f>
           </x14:formula1>
           <xm:sqref>N2:N33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Parametros!$L$2:$L$26</xm:f>
           </x14:formula1>
@@ -1286,7 +1325,738 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7916A9E9-2A23-4520-A279-A5D81BD0E2E5}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43301</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12345</v>
+      </c>
+      <c r="F2" s="2">
+        <f xml:space="preserve"> (C2 - B2)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L2, FIND(" / ", L2) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L2,  LEN(L2) - FIND(" / ", L2) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M2, FIND(" / ", M2) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M2,  LEN(M2) - FIND(" / ", M2) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43301</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="3">
+        <v>54321</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F5" si="0" xml:space="preserve"> (C3 - B3)</f>
+        <v>0.125</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L3, FIND(" / ", L3) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L3,  LEN(L3) - FIND(" / ", L3) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M3, FIND(" / ", M3) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M3,  LEN(M3) - FIND(" / ", M3) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43301</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="3">
+        <v>32145</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L4, FIND(" / ", L4) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L4,  LEN(L4) - FIND(" / ", L4) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M4, FIND(" / ", M4) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="K4" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M4,  LEN(M4) - FIND(" / ", M4) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f ca="1">TODAY()</f>
+        <v>43301</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45321</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L5, FIND(" / ", L5) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L5,  LEN(L5) - FIND(" / ", L5) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M5, FIND(" / ", M5) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M5,  LEN(M5) - FIND(" / ", M5) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f ca="1">TODAY() + 1</f>
+        <v>43302</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="3">
+        <v>12345</v>
+      </c>
+      <c r="F6" s="2">
+        <f xml:space="preserve"> (C6 - B6)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L6, FIND(" / ", L6) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L6,  LEN(L6) - FIND(" / ", L6) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M6, FIND(" / ", M6) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M6,  LEN(M6) - FIND(" / ", M6) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" ref="A7:A9" ca="1" si="1">TODAY() + 1</f>
+        <v>43302</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="3">
+        <v>54321</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F9" si="2" xml:space="preserve"> (C7 - B7)</f>
+        <v>0.125</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L7, FIND(" / ", L7) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L7,  LEN(L7) - FIND(" / ", L7) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M7, FIND(" / ", M7) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M7,  LEN(M7) - FIND(" / ", M7) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>43302</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3">
+        <v>32145</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L8, FIND(" / ", L8) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L8,  LEN(L8) - FIND(" / ", L8) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M8, FIND(" / ", M8) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M8,  LEN(M8) - FIND(" / ", M8) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>43302</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45321</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1875</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(L9, FIND(" / ", L9) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(L9,  LEN(L9) - FIND(" / ", L9) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="J9" s="3">
+        <f>IFERROR(VLOOKUP( LEFT(M9, FIND(" / ", M9) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="3">
+        <f>IFERROR(VLOOKUP( RIGHT(M9,  LEN(M9) - FIND(" / ", M9) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L10, FIND(" / ", L10) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I10" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L10,  LEN(L10) - FIND(" / ", L10) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M10, FIND(" / ", M10) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K10" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M10,  LEN(M10) - FIND(" / ", M10) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L11, FIND(" / ", L11) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I11" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L11,  LEN(L11) - FIND(" / ", L11) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J11" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M11, FIND(" / ", M11) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K11" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M11,  LEN(M11) - FIND(" / ", M11) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L12, FIND(" / ", L12) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I12" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L12,  LEN(L12) - FIND(" / ", L12) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J12" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M12, FIND(" / ", M12) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K12" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M12,  LEN(M12) - FIND(" / ", M12) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L13, FIND(" / ", L13) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I13" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L13,  LEN(L13) - FIND(" / ", L13) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J13" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M13, FIND(" / ", M13) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K13" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M13,  LEN(M13) - FIND(" / ", M13) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L14, FIND(" / ", L14) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I14" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L14,  LEN(L14) - FIND(" / ", L14) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J14" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M14, FIND(" / ", M14) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K14" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M14,  LEN(M14) - FIND(" / ", M14) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L15, FIND(" / ", L15) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I15" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L15,  LEN(L15) - FIND(" / ", L15) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J15" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M15, FIND(" / ", M15) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M15,  LEN(M15) - FIND(" / ", M15) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L16, FIND(" / ", L16) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I16" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L16,  LEN(L16) - FIND(" / ", L16) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J16" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M16, FIND(" / ", M16) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K16" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M16,  LEN(M16) - FIND(" / ", M16) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L17, FIND(" / ", L17) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I17" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L17,  LEN(L17) - FIND(" / ", L17) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J17" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M17, FIND(" / ", M17) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K17" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M17,  LEN(M17) - FIND(" / ", M17) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L18, FIND(" / ", L18) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I18" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L18,  LEN(L18) - FIND(" / ", L18) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J18" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M18, FIND(" / ", M18) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K18" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M18,  LEN(M18) - FIND(" / ", M18) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L19, FIND(" / ", L19) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I19" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L19,  LEN(L19) - FIND(" / ", L19) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J19" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M19, FIND(" / ", M19) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K19" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M19,  LEN(M19) - FIND(" / ", M19) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L20, FIND(" / ", L20) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I20" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L20,  LEN(L20) - FIND(" / ", L20) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J20" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M20, FIND(" / ", M20) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K20" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M20,  LEN(M20) - FIND(" / ", M20) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L21, FIND(" / ", L21) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I21" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L21,  LEN(L21) - FIND(" / ", L21) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J21" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M21, FIND(" / ", M21) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K21" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M21,  LEN(M21) - FIND(" / ", M21) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L22, FIND(" / ", L22) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I22" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L22,  LEN(L22) - FIND(" / ", L22) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J22" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M22, FIND(" / ", M22) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K22" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M22,  LEN(M22) - FIND(" / ", M22) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(L23, FIND(" / ", L23) - 1), Parametros!$A$2:$B$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="I23" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(L23,  LEN(L23) - FIND(" / ", L23) - 2), Parametros!$A$17:$B$25, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="J23" s="3" t="str">
+        <f>IFERROR(VLOOKUP( LEFT(M23, FIND(" / ", M23) - 1), Parametros!$G$2:$H$26, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K23" s="3" t="str">
+        <f>IFERROR(VLOOKUP( RIGHT(M23,  LEN(M23) - FIND(" / ", M23) - 2), Parametros!$G$12:$H$21, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C25B132F-FADE-44D5-BA25-55EC59A8A9B7}">
+          <x14:formula1>
+            <xm:f>Parametros!$L$2:$L$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FFEB9900-8AA5-40E1-9C8C-BF02C7400249}">
+          <x14:formula1>
+            <xm:f>Parametros!$F$2:$F$26</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L33</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1340,7 +2110,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f ca="1">TODAY() - 1</f>
-        <v>42718</v>
+        <v>43300</v>
       </c>
       <c r="B2" s="2">
         <v>0.33333333333333331</v>
@@ -1377,7 +2147,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f ca="1">TODAY() - 1</f>
-        <v>42718</v>
+        <v>43300</v>
       </c>
       <c r="B3" s="2">
         <v>0.54166666666666663</v>
@@ -1414,7 +2184,7 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f ca="1">TODAY()</f>
-        <v>42719</v>
+        <v>43301</v>
       </c>
       <c r="B4" s="2">
         <v>0.33333333333333331</v>
@@ -1451,7 +2221,7 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f ca="1">TODAY()</f>
-        <v>42719</v>
+        <v>43301</v>
       </c>
       <c r="B5" s="2">
         <v>0.54166666666666663</v>
@@ -1534,13 +2304,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Parametros!$F$2:$F$26</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Parametros!$L$2:$L$26</xm:f>
           </x14:formula1>
@@ -1552,8 +2322,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1633,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D2, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E2, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" ref="F2:F26" si="0" xml:space="preserve"> IFERROR( VLOOKUP(D2, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E2, $B$17:$C$25, 2, FALSE), "")</f>
         <v>Projeto 1 / Sistema 1</v>
       </c>
       <c r="G2" s="4" t="str">
@@ -1653,13 +2423,13 @@
         <v>1</v>
       </c>
       <c r="L2" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J2, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K2, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" ref="L2:L26" si="1" xml:space="preserve"> IFERROR( VLOOKUP(J2, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K2, $H$16:$I$21, 2, FALSE), "")</f>
         <v>Desenv. / Melhoria</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f t="shared" ref="A3:A10" si="0">C3</f>
+        <f t="shared" ref="A3:A10" si="2">C3</f>
         <v>Projeto 2</v>
       </c>
       <c r="B3" s="11">
@@ -1675,11 +2445,11 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D3, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E3, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 1 / Sistema 2</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f t="shared" ref="G3:G20" si="1">I3</f>
+        <f t="shared" ref="G3:G14" si="3">I3</f>
         <v>Testes</v>
       </c>
       <c r="H3" s="4">
@@ -1695,13 +2465,13 @@
         <v>2</v>
       </c>
       <c r="L3" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J3, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K3, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Desenv. / Projeto</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Projeto 3</v>
       </c>
       <c r="B4" s="11">
@@ -1717,11 +2487,11 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D4, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E4, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 1 / Sistema 3</v>
       </c>
       <c r="G4" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Especificações</v>
       </c>
       <c r="H4" s="4">
@@ -1737,13 +2507,13 @@
         <v>3</v>
       </c>
       <c r="L4" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J4, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K4, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Desenv. / Correção</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Projeto 4</v>
       </c>
       <c r="B5" s="11">
@@ -1759,11 +2529,11 @@
         <v>4</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D5, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E5, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 1 / Sistema 4</v>
       </c>
       <c r="G5" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Suporte</v>
       </c>
       <c r="H5" s="4">
@@ -1779,13 +2549,13 @@
         <v>19</v>
       </c>
       <c r="L5" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J5, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K5, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Desenv. / Merge</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Projeto 5</v>
       </c>
       <c r="B6" s="11">
@@ -1801,11 +2571,11 @@
         <v>5</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D6, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E6, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 1 / Sistema 5</v>
       </c>
       <c r="G6" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Análises</v>
       </c>
       <c r="H6" s="4">
@@ -1821,13 +2591,13 @@
         <v>20</v>
       </c>
       <c r="L6" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J6, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K6, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Desenv. / Deploy</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B7" s="11"/>
@@ -1839,11 +2609,11 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D7, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E7, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 2 / Sistema 1</v>
       </c>
       <c r="G7" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Planejamento / Reuniões</v>
       </c>
       <c r="H7" s="4">
@@ -1859,13 +2629,13 @@
         <v>1</v>
       </c>
       <c r="L7" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J7, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K7, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Testes / Melhoria</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B8" s="11"/>
@@ -1877,11 +2647,11 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D8, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E8, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 2 / Sistema 2</v>
       </c>
       <c r="G8" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Ativ. Administrativas</v>
       </c>
       <c r="H8" s="4">
@@ -1897,13 +2667,13 @@
         <v>2</v>
       </c>
       <c r="L8" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J8, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K8, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Testes / Projeto</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B9" s="12"/>
@@ -1915,11 +2685,11 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D9, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E9, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 2 / Sistema 3</v>
       </c>
       <c r="G9" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Treinamento</v>
       </c>
       <c r="H9" s="4">
@@ -1935,13 +2705,13 @@
         <v>3</v>
       </c>
       <c r="L9" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J9, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K9, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Testes / Correção</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B10" s="12"/>
@@ -1953,11 +2723,11 @@
         <v>4</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D10, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E10, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 2 / Sistema 4</v>
       </c>
       <c r="G10" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Deploy QA</v>
       </c>
       <c r="H10" s="4">
@@ -1973,7 +2743,7 @@
         <v>19</v>
       </c>
       <c r="L10" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J10, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K10, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Testes / Merge</v>
       </c>
     </row>
@@ -1985,11 +2755,11 @@
         <v>5</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D11, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E11, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 2 / Sistema 5</v>
       </c>
       <c r="G11" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Ausências</v>
       </c>
       <c r="H11" s="4">
@@ -2005,7 +2775,7 @@
         <v>20</v>
       </c>
       <c r="L11" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J11, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K11, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Testes / Deploy</v>
       </c>
     </row>
@@ -2017,11 +2787,11 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D12, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E12, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 3 / Sistema 1</v>
       </c>
       <c r="G12" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Ativ. Oper. Indevida</v>
       </c>
       <c r="H12" s="4">
@@ -2037,7 +2807,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J12, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K12, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Especificações / Melhoria</v>
       </c>
     </row>
@@ -2049,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D13, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E13, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 3 / Sistema 2</v>
       </c>
       <c r="G13" s="4">
@@ -2063,7 +2833,7 @@
         <v>2</v>
       </c>
       <c r="L13" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J13, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K13, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Especificações / Projeto</v>
       </c>
     </row>
@@ -2075,11 +2845,11 @@
         <v>3</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D14, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E14, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 3 / Sistema 3</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J14" s="13">
@@ -2089,7 +2859,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J14, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K14, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Especificações / Correção</v>
       </c>
     </row>
@@ -2101,7 +2871,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D15, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E15, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 3 / Sistema 4</v>
       </c>
       <c r="J15" s="13">
@@ -2111,13 +2881,13 @@
         <v>19</v>
       </c>
       <c r="L15" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J15, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K15, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Especificações / Merge</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="str">
-        <f t="shared" ref="A16:A25" si="2">C16</f>
+        <f t="shared" ref="A16:A25" si="4">C16</f>
         <v>Sistemas</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -2133,11 +2903,11 @@
         <v>5</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D16, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E16, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 3 / Sistema 5</v>
       </c>
       <c r="G16" s="17" t="str">
-        <f>I16</f>
+        <f t="shared" ref="G16:G21" si="5">I16</f>
         <v>Atividade</v>
       </c>
       <c r="H16" s="10" t="s">
@@ -2153,13 +2923,13 @@
         <v>20</v>
       </c>
       <c r="L16" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J16, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K16, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Especificações / Deploy</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sistema 1</v>
       </c>
       <c r="B17" s="11">
@@ -2175,11 +2945,11 @@
         <v>1</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D17, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E17, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 4 / Sistema 1</v>
       </c>
       <c r="G17" s="4" t="str">
-        <f>I17</f>
+        <f t="shared" si="5"/>
         <v>Melhoria</v>
       </c>
       <c r="H17" s="4">
@@ -2195,13 +2965,13 @@
         <v>1</v>
       </c>
       <c r="L17" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J17, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K17, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Suporte / Melhoria</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sistema 2</v>
       </c>
       <c r="B18" s="11">
@@ -2217,11 +2987,11 @@
         <v>2</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D18, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E18, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 4 / Sistema 2</v>
       </c>
       <c r="G18" s="4" t="str">
-        <f>I18</f>
+        <f t="shared" si="5"/>
         <v>Projeto</v>
       </c>
       <c r="H18" s="4">
@@ -2237,13 +3007,13 @@
         <v>2</v>
       </c>
       <c r="L18" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J18, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K18, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Suporte / Projeto</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sistema 3</v>
       </c>
       <c r="B19" s="11">
@@ -2259,11 +3029,11 @@
         <v>3</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D19, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E19, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 4 / Sistema 3</v>
       </c>
       <c r="G19" s="4" t="str">
-        <f>I19</f>
+        <f t="shared" si="5"/>
         <v>Correção</v>
       </c>
       <c r="H19" s="4">
@@ -2279,13 +3049,13 @@
         <v>3</v>
       </c>
       <c r="L19" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J19, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K19, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Suporte / Correção</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sistema 4</v>
       </c>
       <c r="B20" s="11">
@@ -2301,11 +3071,11 @@
         <v>4</v>
       </c>
       <c r="F20" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D20, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E20, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 4 / Sistema 4</v>
       </c>
       <c r="G20" s="4" t="str">
-        <f>I20</f>
+        <f t="shared" si="5"/>
         <v>Merge</v>
       </c>
       <c r="H20" s="4">
@@ -2321,13 +3091,13 @@
         <v>19</v>
       </c>
       <c r="L20" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J20, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K20, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Suporte / Merge</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Sistema 5</v>
       </c>
       <c r="B21" s="11">
@@ -2343,11 +3113,11 @@
         <v>5</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D21, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E21, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 4 / Sistema 5</v>
       </c>
       <c r="G21" s="4" t="str">
-        <f>I21</f>
+        <f t="shared" si="5"/>
         <v>Deploy</v>
       </c>
       <c r="H21" s="4">
@@ -2363,13 +3133,13 @@
         <v>20</v>
       </c>
       <c r="L21" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J21, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K21, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Suporte / Deploy</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B22" s="14"/>
@@ -2381,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D22, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E22, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 5 / Sistema 1</v>
       </c>
       <c r="J22" s="13">
@@ -2391,13 +3161,13 @@
         <v>1</v>
       </c>
       <c r="L22" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J22, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K22, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Análises / Melhoria</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B23" s="14"/>
@@ -2409,7 +3179,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D23, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E23, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 5 / Sistema 2</v>
       </c>
       <c r="J23" s="13">
@@ -2419,13 +3189,13 @@
         <v>2</v>
       </c>
       <c r="L23" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J23, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K23, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Análises / Projeto</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B24" s="14"/>
@@ -2437,7 +3207,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D24, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E24, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 5 / Sistema 3</v>
       </c>
       <c r="J24" s="13">
@@ -2447,13 +3217,13 @@
         <v>3</v>
       </c>
       <c r="L24" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J24, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K24, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Análises / Correção</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B25" s="14"/>
@@ -2465,7 +3235,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D25, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E25, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 5 / Sistema 4</v>
       </c>
       <c r="J25" s="13">
@@ -2475,7 +3245,7 @@
         <v>19</v>
       </c>
       <c r="L25" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J25, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K25, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Análises / Merge</v>
       </c>
     </row>
@@ -2489,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(D26, $B$2:$C$10, 2, FALSE) &amp; " / " &amp; VLOOKUP(E26, $B$17:$C$25, 2, FALSE), "")</f>
+        <f t="shared" si="0"/>
         <v>Projeto 5 / Sistema 5</v>
       </c>
       <c r="J26" s="13">
@@ -2499,7 +3269,7 @@
         <v>20</v>
       </c>
       <c r="L26" s="4" t="str">
-        <f xml:space="preserve"> IFERROR( VLOOKUP(J26, $H$2:$I$13, 2, FALSE) &amp; " / " &amp; VLOOKUP(K26, $H$16:$I$21, 2, FALSE), "")</f>
+        <f t="shared" si="1"/>
         <v>Análises / Deploy</v>
       </c>
     </row>

</xml_diff>